<commit_message>
avances con todo, poniendo al dia la rama
</commit_message>
<xml_diff>
--- a/Proyectos Evaluados/Leon/Antecedentes PF - León de Gules II_V1.xlsx
+++ b/Proyectos Evaluados/Leon/Antecedentes PF - León de Gules II_V1.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nayal\Desktop\ejecucion-modelos\Proyectos Evaluados\Leon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C106C84C-5BFF-41C9-A59C-6937FC58D7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A521538E-0BBA-4B78-9BCF-FA65BA87BC61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{A8E2847A-B53C-4F40-AC56-E093DD92F3C8}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="2" activeTab="3" xr2:uid="{A8E2847A-B53C-4F40-AC56-E093DD92F3C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Caso PMG" sheetId="1" r:id="rId1"/>
     <sheet name="Perfil 10,611MWp" sheetId="4" r:id="rId2"/>
     <sheet name="Resultados" sheetId="5" r:id="rId3"/>
+    <sheet name="Resultados Sensibilidades" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
   <si>
     <t>Nodo de Referencia (DNV)</t>
   </si>
@@ -377,6 +378,96 @@
       <t>, BESS 9 MW 36 MWh (4 hrs)</t>
     </r>
   </si>
+  <si>
+    <t>MEJOR CASO: PV 10,611 MWp, BESS 9 MW 27 MWh (3 hrs)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">PV 10,611 MWp, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>BESS 9 MW 27 MWh (3 hrs) - EPC 0,12</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">PV 10,611 MWp, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>BESS 9 MW 27 MWh (3 hrs) - EPC 0,14</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">PV 10,611 MWp, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>BESS 9 MW 27 MWh (3 hrs) - EPC 0,16</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">PV 10,611 MWp, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>BESS 9 MW 27 MWh (3 hrs) - EPC 0,18</t>
+    </r>
+  </si>
+  <si>
+    <t>PV 10,611 MWp, BESS 9 MW 27 MWh (3 hrs) - EPC 0,20</t>
+  </si>
 </sst>
 </file>
 
@@ -584,13 +675,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -649,6 +741,12 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -676,18 +774,19 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="10" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="5" fillId="6" borderId="6" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{9AC97E2C-F70C-4CD1-85D3-1EC36D4C1456}"/>
     <cellStyle name="Notas" xfId="1" builtinId="10"/>
     <cellStyle name="Note 2" xfId="2" xr:uid="{6706319B-B46B-475C-93C0-D2080348B348}"/>
+    <cellStyle name="Porcentaje" xfId="4" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1022,7 +1121,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1034,12 +1133,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -1056,7 +1155,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="27" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1070,7 +1169,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="25"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1082,7 +1181,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="25"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="2" t="s">
         <v>37</v>
       </c>
@@ -1094,7 +1193,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="25"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1106,7 +1205,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="26" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1120,7 +1219,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="24"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
@@ -1132,7 +1231,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="24"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
@@ -1158,7 +1257,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="22" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1172,7 +1271,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
@@ -1184,7 +1283,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="21"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="3" t="s">
         <v>27</v>
       </c>
@@ -1196,7 +1295,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
@@ -1208,7 +1307,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="28" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1222,7 +1321,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="27"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="2" t="s">
         <v>13</v>
       </c>
@@ -1234,7 +1333,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="27"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
@@ -1246,7 +1345,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="27"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1258,7 +1357,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="27"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="2" t="s">
         <v>23</v>
       </c>
@@ -1270,7 +1369,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="27"/>
+      <c r="A20" s="29"/>
       <c r="B20" s="2" t="s">
         <v>24</v>
       </c>
@@ -1282,7 +1381,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="27"/>
+      <c r="A21" s="29"/>
       <c r="B21" s="2" t="s">
         <v>25</v>
       </c>
@@ -1294,7 +1393,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="28"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="2" t="s">
         <v>26</v>
       </c>
@@ -1306,7 +1405,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="22" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1320,7 +1419,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="21"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="3" t="s">
         <v>29</v>
       </c>
@@ -1333,7 +1432,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="22"/>
+      <c r="A25" s="24"/>
       <c r="B25" s="3" t="s">
         <v>30</v>
       </c>
@@ -71474,8 +71573,8 @@
   </sheetPr>
   <dimension ref="B2:G11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -71588,22 +71687,22 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="21">
         <v>6.6199999999999995E-2</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="21">
         <v>7.51E-2</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="20">
         <v>0.46</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="20">
         <v>9.9</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="20">
         <v>68.8</v>
       </c>
     </row>
@@ -71686,6 +71785,195 @@
       <c r="G11" s="13">
         <v>72.5</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93D8BA27-3691-489B-BF60-B85326B07C38}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="B2:G11"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.88671875" style="17" customWidth="1"/>
+    <col min="2" max="2" width="54" style="17" customWidth="1"/>
+    <col min="3" max="7" width="20.5546875" style="17" customWidth="1"/>
+    <col min="8" max="8" width="78.5546875" style="17" customWidth="1"/>
+    <col min="9" max="16384" width="8.6640625" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="14">
+        <v>6.5799999999999997E-2</v>
+      </c>
+      <c r="D3" s="14">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E3" s="13">
+        <v>0.49</v>
+      </c>
+      <c r="F3" s="13">
+        <v>9.9</v>
+      </c>
+      <c r="G3" s="13">
+        <v>65.400000000000006</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="19"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+    </row>
+    <row r="5" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="14">
+        <v>0.10580000000000001</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0.11210000000000001</v>
+      </c>
+      <c r="E5" s="13">
+        <v>3.41</v>
+      </c>
+      <c r="F5" s="13">
+        <v>3.4</v>
+      </c>
+      <c r="G5" s="13">
+        <v>52.4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="16">
+        <v>9.5699999999999993E-2</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0.1026</v>
+      </c>
+      <c r="E6" s="15">
+        <v>2.76</v>
+      </c>
+      <c r="F6" s="15">
+        <v>8.1</v>
+      </c>
+      <c r="G6" s="15">
+        <v>55.3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="32">
+        <v>8.6400000000000005E-2</v>
+      </c>
+      <c r="D7" s="32">
+        <v>9.3899999999999997E-2</v>
+      </c>
+      <c r="E7" s="13">
+        <v>2.11</v>
+      </c>
+      <c r="F7" s="13">
+        <v>8.6</v>
+      </c>
+      <c r="G7" s="13">
+        <v>58.1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="16">
+        <v>7.7799999999999994E-2</v>
+      </c>
+      <c r="D8" s="16">
+        <v>8.5900000000000004E-2</v>
+      </c>
+      <c r="E8" s="15">
+        <v>1.46</v>
+      </c>
+      <c r="F8" s="15">
+        <v>9.1</v>
+      </c>
+      <c r="G8" s="15">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="14">
+        <v>6.9699999999999998E-2</v>
+      </c>
+      <c r="D9" s="14">
+        <v>7.85E-2</v>
+      </c>
+      <c r="E9" s="13">
+        <v>0.81</v>
+      </c>
+      <c r="F9" s="13">
+        <v>9.6</v>
+      </c>
+      <c r="G9" s="13">
+        <v>63.9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="19"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+    </row>
+    <row r="11" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="13"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>